<commit_message>
Simplified DigitalShares contract Refactored to use small amount of gas on all functions
</commit_message>
<xml_diff>
--- a/DigitalShare Stats.xlsx
+++ b/DigitalShare Stats.xlsx
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,18 +440,18 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -459,7 +459,7 @@
         <v>646811</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -467,7 +467,7 @@
         <v>67557</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -475,7 +475,7 @@
         <v>568877</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -483,7 +483,7 @@
         <v>47983</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -491,7 +491,7 @@
         <v>33127</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -508,7 +508,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -524,8 +524,11 @@
       <c r="E10">
         <v>1392227</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>452790</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -540,6 +543,9 @@
       </c>
       <c r="E11">
         <v>1825566</v>
+      </c>
+      <c r="F11">
+        <v>1438649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updated article - Reviewed DigitalShares contract
</commit_message>
<xml_diff>
--- a/DigitalShare Stats.xlsx
+++ b/DigitalShare Stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DigitalShare</t>
-  </si>
-  <si>
-    <t>initialize</t>
-  </si>
-  <si>
-    <t>addShare</t>
-  </si>
-  <si>
-    <t>sendShares</t>
-  </si>
-  <si>
-    <t>distributeDividends</t>
   </si>
   <si>
     <t>Method/gas</t>
@@ -51,16 +39,13 @@
     <t>withdraw</t>
   </si>
   <si>
-    <t>registerStock</t>
-  </si>
-  <si>
-    <t>unregisterStock</t>
+    <t>distribute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,115 +422,60 @@
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>74320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>646811</v>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>67557</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>568877</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>47983</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>33127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>100</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>54247</v>
-      </c>
-      <c r="C10">
-        <v>92093</v>
-      </c>
-      <c r="D10">
-        <v>208283</v>
-      </c>
-      <c r="E10">
-        <v>1392227</v>
-      </c>
-      <c r="F10">
-        <v>452790</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>61332</v>
-      </c>
-      <c r="C11">
-        <v>92357</v>
-      </c>
-      <c r="D11">
-        <v>236166</v>
-      </c>
-      <c r="E11">
-        <v>1825566</v>
-      </c>
-      <c r="F11">
-        <v>1438649</v>
+        <v>69511</v>
+      </c>
+      <c r="C6">
+        <v>80482</v>
+      </c>
+      <c r="D6">
+        <v>190192</v>
+      </c>
+      <c r="E6">
+        <v>1287292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>